<commit_message>
Abstract shipment data to locate respective sheet WIP.
</commit_message>
<xml_diff>
--- a/separated_us_express_rates.xlsx
+++ b/separated_us_express_rates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtrav\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtrav\dmg_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134D5B42-73F0-4DFA-AAE8-D0EB4EFC871E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A8E329-C5AB-4542-AA79-B9FDB45E6540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="747" xr2:uid="{CFA89F8F-38C2-474B-9658-B8D182092B59}"/>
+    <workbookView xWindow="-28920" yWindow="-3615" windowWidth="29040" windowHeight="15840" tabRatio="747" activeTab="2" xr2:uid="{CFA89F8F-38C2-474B-9658-B8D182092B59}"/>
   </bookViews>
   <sheets>
     <sheet name="FedEx First Overnight®" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="MW FedEx 2Day® A.M." sheetId="11" r:id="rId11"/>
     <sheet name="MW FedEx 2Day®" sheetId="12" r:id="rId12"/>
     <sheet name="MW FedEx Express Saver®" sheetId="13" r:id="rId13"/>
-    <sheet name="MWIntra-HawaiiFedExPriorityON®" sheetId="14" r:id="rId14"/>
+    <sheet name="MWIntra-HawaiiFedExPriorityON" sheetId="14" r:id="rId14"/>
     <sheet name="FedEx First Overnight® Freight" sheetId="17" r:id="rId15"/>
     <sheet name="FedEx 1Day® Freight" sheetId="18" r:id="rId16"/>
     <sheet name="FedEx 2Day® Freight" sheetId="19" r:id="rId17"/>
@@ -1067,7 +1067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F19A77-2D09-4445-9A0B-A4A1E97988D1}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6416,7 +6416,7 @@
   <dimension ref="A7:K12"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6620,7 +6620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADC67F1-79FE-4C1F-A24E-54E2436E363F}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6823,7 +6825,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE72C7D8-A6BA-460C-8968-05E3490F227C}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -7231,7 +7235,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695C9F6B-CEAE-4A2E-9C97-A8793740B125}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -7274,7 +7280,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC5879A-1A49-454A-B822-262C51DD3150}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7517,7 +7525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A4AF85-7394-4D06-87A1-37F2D7FBE7C9}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -7755,7 +7765,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BC203C-048F-489C-8D47-171992E7D34E}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -7993,7 +8005,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58916E4A-699A-4309-A88B-CA03D1D1D3B7}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -13522,7 +13536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D059C905-0282-41DD-92B4-6E4A7DFA186A}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -29566,7 +29582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7A0CE9-C457-4B0B-9E9B-CCF0567B4A60}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -34914,7 +34932,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5915C6F-0FC8-41AD-9AE4-C6ED33C8D1CC}">
   <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -36149,7 +36169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB014F2-B709-483F-8278-FCBD8EE7C73B}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -36353,7 +36375,7 @@
   <dimension ref="A4:K9"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Auto generate OTPUB and error handling.
</commit_message>
<xml_diff>
--- a/separated_us_express_rates.xlsx
+++ b/separated_us_express_rates.xlsx
@@ -8,29 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtrav\dmg_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52F7EA6-BFEE-47FA-9D22-CFC50DD10656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A2B1BC-AE2A-49A7-AAE5-285AA6D00B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="747" firstSheet="15" activeTab="18" xr2:uid="{CFA89F8F-38C2-474B-9658-B8D182092B59}"/>
+    <workbookView xWindow="28680" yWindow="-1560" windowWidth="29040" windowHeight="15840" tabRatio="747" firstSheet="4" activeTab="6" xr2:uid="{CFA89F8F-38C2-474B-9658-B8D182092B59}"/>
   </bookViews>
   <sheets>
-    <sheet name="FedEx First Overnight®" sheetId="1" r:id="rId1"/>
-    <sheet name="FedEx Priority Overnight®" sheetId="2" r:id="rId2"/>
-    <sheet name="FedEx Standard Overnight®" sheetId="3" r:id="rId3"/>
-    <sheet name="FedEx 2Day® A.M." sheetId="4" r:id="rId4"/>
-    <sheet name="FedEx 2Day®" sheetId="5" r:id="rId5"/>
-    <sheet name="FedEx Express Saver®" sheetId="6" r:id="rId6"/>
+    <sheet name="FedEx First Overnight" sheetId="1" r:id="rId1"/>
+    <sheet name="FedEx Priority Overnight" sheetId="2" r:id="rId2"/>
+    <sheet name="FedEx Standard Overnight" sheetId="3" r:id="rId3"/>
+    <sheet name="FedEx 2Day A.M." sheetId="4" r:id="rId4"/>
+    <sheet name="FedEx 2Day" sheetId="5" r:id="rId5"/>
+    <sheet name="FedEx Express Saver" sheetId="6" r:id="rId6"/>
     <sheet name="Intra-Hawaii Standard List Rate" sheetId="7" r:id="rId7"/>
-    <sheet name="MW FedEx First Overnight®" sheetId="8" r:id="rId8"/>
-    <sheet name="MW FedEx Priority Overnight®" sheetId="9" r:id="rId9"/>
-    <sheet name="MW FedEx Standard Overnight®" sheetId="10" r:id="rId10"/>
-    <sheet name="MW FedEx 2Day® A.M." sheetId="11" r:id="rId11"/>
-    <sheet name="MW FedEx 2Day®" sheetId="12" r:id="rId12"/>
-    <sheet name="MW FedEx Express Saver®" sheetId="13" r:id="rId13"/>
+    <sheet name="MW FedEx First Overnight" sheetId="8" r:id="rId8"/>
+    <sheet name="MW FedEx Priority Overnight" sheetId="9" r:id="rId9"/>
+    <sheet name="MW FedEx Standard Overnight" sheetId="10" r:id="rId10"/>
+    <sheet name="MW FedEx 2Day A.M." sheetId="11" r:id="rId11"/>
+    <sheet name="MW FedEx 2Day" sheetId="12" r:id="rId12"/>
+    <sheet name="MW FedEx Express Saver" sheetId="13" r:id="rId13"/>
     <sheet name="MWIntra-HawaiiFedExPriorityON" sheetId="14" r:id="rId14"/>
-    <sheet name="FedEx First Overnight® Freight" sheetId="17" r:id="rId15"/>
-    <sheet name="FedEx 1Day® Freight" sheetId="18" r:id="rId16"/>
-    <sheet name="FedEx 2Day® Freight" sheetId="19" r:id="rId17"/>
-    <sheet name="FedEx 3Day® Freight" sheetId="20" r:id="rId18"/>
+    <sheet name="FedEx First Overnight Freight" sheetId="17" r:id="rId15"/>
+    <sheet name="FedEx 1Day Freight" sheetId="18" r:id="rId16"/>
+    <sheet name="FedEx 2Day Freight" sheetId="19" r:id="rId17"/>
+    <sheet name="FedEx 3Day Freight" sheetId="20" r:id="rId18"/>
     <sheet name="FHD Ground" sheetId="21" r:id="rId19"/>
     <sheet name="FHD Ground Canada" sheetId="22" r:id="rId20"/>
   </sheets>
@@ -7942,7 +7942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64432EBE-ABE2-44D2-AB97-222B7EA0E804}">
   <dimension ref="A1:P153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -44099,7 +44099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5915C6F-0FC8-41AD-9AE4-C6ED33C8D1CC}">
   <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DIM calc error handling WIP.
</commit_message>
<xml_diff>
--- a/separated_us_express_rates.xlsx
+++ b/separated_us_express_rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtrav\dmg_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A2B1BC-AE2A-49A7-AAE5-285AA6D00B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFBCF2B-B634-4F66-AB10-83DE6C99C907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1560" windowWidth="29040" windowHeight="15840" tabRatio="747" firstSheet="4" activeTab="6" xr2:uid="{CFA89F8F-38C2-474B-9658-B8D182092B59}"/>
+    <workbookView xWindow="28680" yWindow="-1560" windowWidth="29040" windowHeight="15840" tabRatio="747" activeTab="1" xr2:uid="{CFA89F8F-38C2-474B-9658-B8D182092B59}"/>
   </bookViews>
   <sheets>
     <sheet name="FedEx First Overnight" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="30">
   <si>
     <t>Zones</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>From Hawaii</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
@@ -598,6 +601,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -918,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F19A77-2D09-4445-9A0B-A4A1E97988D1}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -6670,7 +6676,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE72C7D8-A6BA-460C-8968-05E3490F227C}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
@@ -6851,6 +6857,11 @@
       </c>
       <c r="K5" s="37">
         <v>3.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -15554,8 +15565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A46695-8485-4D73-8F3C-521EDD6829C5}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20930,7 +20941,7 @@
   <dimension ref="A1:C151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22606,7 +22617,7 @@
   <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44099,7 +44110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5915C6F-0FC8-41AD-9AE4-C6ED33C8D1CC}">
   <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FedEx Envelope price calc, irregular zone handling for ground shipments.
</commit_message>
<xml_diff>
--- a/separated_us_express_rates.xlsx
+++ b/separated_us_express_rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtrav\dmg_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFBCF2B-B634-4F66-AB10-83DE6C99C907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4709C2DB-FDBB-4E80-8906-22223928260C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1560" windowWidth="29040" windowHeight="15840" tabRatio="747" activeTab="1" xr2:uid="{CFA89F8F-38C2-474B-9658-B8D182092B59}"/>
+    <workbookView xWindow="28680" yWindow="-1560" windowWidth="29040" windowHeight="15840" tabRatio="747" firstSheet="13" activeTab="19" xr2:uid="{CFA89F8F-38C2-474B-9658-B8D182092B59}"/>
   </bookViews>
   <sheets>
     <sheet name="FedEx First Overnight" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
@@ -601,9 +601,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -925,7 +922,7 @@
   <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6860,7 +6857,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -7954,7 +7951,7 @@
   <dimension ref="A1:P153"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15565,7 +15562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A46695-8485-4D73-8F3C-521EDD6829C5}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -20940,7 +20937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FA3913E-A60E-4E37-935E-C6FE89B9D59F}">
   <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>